<commit_message>
We can check which of all sensors is online!
</commit_message>
<xml_diff>
--- a/arduino/Таблица датчиков.xlsx
+++ b/arduino/Таблица датчиков.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Номер датчика</t>
   </si>
@@ -31,63 +31,113 @@
     <t xml:space="preserve">28 FF 90 25 A4 16 4 41</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 144 37 164 22 4 65</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 20 96 A4 16 4 17</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 32 150 164 22 4 23</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 42 47 A4 16 4 B</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 66 71 164 22 4 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF A1 9B A4 16 5 D2</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 161 155 164 22 5 210</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF BB D A4 16 5 FB</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 187 13 164 22 5 251</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 76 A1 A4 16 5 8E</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 118 161 164 22 5 142</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 97 48 A4 16 4 1D</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 151 72 164 22 4 29</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 15 B A4 16 5 63</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 21 11 164 22 5 99</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 5B 9C A4 16 5 4F</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 91 156 164 22 5 79</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 72 60 A4 16 4 79</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 114 96 164 22 4 121</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 4A 56 A4 16 4 82</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 74 86 164 22 4 130</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 11 4E A4 16 4 43</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 17 78 164 22 4 67</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 2B 83 A4 16 4 DE</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 43 131 164 22 4 222</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 7 94 A4 16 4 B9</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 7 148 164 22 4 185</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF B2 C A4 16 5 87</t>
   </si>
   <si>
+    <t xml:space="preserve">40 255 178 12 164 22 5 135</t>
+  </si>
+  <si>
     <t xml:space="preserve">28 FF 76 E0 94 16 4 61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 255 118 224 148 22 4 97</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,8 +197,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,17 +223,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,13 +252,19 @@
       <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,7 +272,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,7 +283,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +294,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,7 +305,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -243,7 +316,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,7 +327,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,7 +338,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,7 +349,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +360,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +371,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,7 +382,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,7 +393,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +404,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,7 +415,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>